<commit_message>
add azure cognitive and refactor main code
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -359,309 +359,514 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Date</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Before Breakfast</t>
+          <t xml:space="preserve"> Before</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Breakfast</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t xml:space="preserve"> After Breakfast</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Before Lunch</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> After Lunch</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Before Dinner</t>
+          <t xml:space="preserve"> Before</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> After Dinner</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ot /OL'20</t>
+          <t xml:space="preserve"> x0</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> +9. LY</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 59, 44</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> yO. 65</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sl té</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> KA AC)</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> aa
-«O
-W&gt;</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OL!
-‘01 {20</t>
+          <t xml:space="preserve"> O41 Oar</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 29 EC</t>
+          <t xml:space="preserve"> 4O)</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> E263</t>
+          <t xml:space="preserve"> 29</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> L443</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Q)
-yy
-A&gt;</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> F2.64</t>
+          <t xml:space="preserve"> £0</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OL?</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> t&amp;</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ae AL)</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FO 65</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> C4/O1 20</t>
+          <t xml:space="preserve"> 2</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> §2.. 63</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5” 40</t>
+          <t xml:space="preserve"> 60</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 59. 43</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 5A. 4 +</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CA. +6</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OL, [01, 20</t>
+          <t xml:space="preserve"> ie ZO</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> sO. ©5</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 62.64</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> G1. ©</t>
+          <t xml:space="preserve"> 40</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Random</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Text</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 549 Lk</t>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 59 4</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 54 Ly Fe</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> oA. +6</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 05 01[70</t>
+          <t xml:space="preserve"> OL 1 | 20</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> GL .+G6</t>
+          <t xml:space="preserve"> ‘O</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 3 4F</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> bh. 40</t>
+          <t xml:space="preserve"> 64</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1 A:
--</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> £0.65</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ah
-oO</t>
+          <t xml:space="preserve"> +6</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Random</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tex</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 06/01/20</t>
+          <t xml:space="preserve"> O4 |</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 62 .L)</t>
+          <t xml:space="preserve"> Gt</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> +6</t>
+          <t xml:space="preserve"> AG</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on K
-9g</t>
+          <t xml:space="preserve"> A</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> FO. Ob</t>
+          <t xml:space="preserve"> -s</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> J)
-1
-.
-f
-4
-v</t>
+          <t xml:space="preserve"> pe)
+Ly</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> L5-6 F</t>
+          <t xml:space="preserve"> 40)</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 4</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> FQ</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> a</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OF/O1/20</t>
+          <t xml:space="preserve"> BB /6 VS</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 59 43</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> £8. 99</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OL. 42</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Li&amp; 92.</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.63</t>
+          <t xml:space="preserve"> AK</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> §. 3]</t>
+          <t xml:space="preserve"> QB?</t>
+        </is>
+      </c>
+      <c r="H8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> fO</t>
+        </is>
+      </c>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 53</t>
+        </is>
+      </c>
+      <c r="K8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> b- +</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> OF [/O1L[20</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 59</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AS</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> he</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="G9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="H9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> LS</t>
+        </is>
+      </c>
+      <c r="I9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="J9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 64</t>
+        </is>
+      </c>
+      <c r="K9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 54</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adjust border extraction to be less noisy
</commit_message>
<xml_diff>
--- a/output/output.xlsx
+++ b/output/output.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -359,514 +359,303 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Before</t>
+          <t xml:space="preserve"> Before Breakfast</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Breakfast</t>
+          <t xml:space="preserve"> After Breakfast</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> After Breakfast</t>
+          <t xml:space="preserve"> Before Lunch</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> After Lunch</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Before</t>
+          <t xml:space="preserve"> Before Dinner</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> After Dinner</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> x0</t>
+          <t xml:space="preserve"> O4/OL/30</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 49. 29</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 59. 44</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> yO. 65</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> sl té</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> KA AC)</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> TO.¢6S</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> O41 Oar</t>
+          <t xml:space="preserve"> 02 {04/20</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 4O)</t>
+          <t xml:space="preserve"> 29.€C</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 29</t>
+          <t xml:space="preserve"> at)
+|
+iY</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> L443</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> CN
+Y
+CY)</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> £0</t>
+          <t xml:space="preserve"> ol)
+F2.G</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> t&amp;</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ae AL)</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FO 65</t>
+          <t xml:space="preserve"> OL U2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2</t>
+          <t xml:space="preserve"> C4/OL{20</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> §2.. 63</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 60</t>
+          <t xml:space="preserve"> 54 40</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 82.64</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 59. 43</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> In. Ly
+~</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> A 4G</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ie ZO</t>
+          <t xml:space="preserve"> 0L1 [01] 20</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> ¥0. ©5</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 62
+62</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 40</t>
+          <t xml:space="preserve"> G1. +6</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Random</t>
         </is>
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Text</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 59 4</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 54 Ly Fe</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> oA. +6</t>
+          <t xml:space="preserve"> 549 Lk</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> OL 1 | 20</t>
+          <t xml:space="preserve"> 05/01/20</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ‘O</t>
+          <t xml:space="preserve"> GL -.46</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 3 4F</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 64</t>
+          <t xml:space="preserve"> bh. 40</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 55.45%</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> FO.eE4</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> +6</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Random</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tex</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> AL.2%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> O4 |</t>
+          <t xml:space="preserve"> 06/01/20</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gt</t>
+          <t xml:space="preserve"> 62 ul</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AG</t>
+          <t xml:space="preserve"> +6</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A</t>
+          <t xml:space="preserve"> 4. SZ</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> -s</t>
+          <t xml:space="preserve"> §O. &amp;4</t>
         </is>
       </c>
       <c r="F7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> pe)
-Ly</t>
+          <t xml:space="preserve"> 562.4]</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 40)</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> A</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 4</t>
-        </is>
-      </c>
-      <c r="J7" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> FQ</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> a</t>
+          <t xml:space="preserve"> L5-6 F</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> BB /6 VS</t>
+          <t xml:space="preserve"> OF/O4L[20</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> 59.43</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> AE, AI</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> Of. 42</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t xml:space="preserve"> L&amp; 97</t>
         </is>
       </c>
       <c r="F8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> AK</t>
+          <t xml:space="preserve"> 2.63</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> QB?</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fO</t>
-        </is>
-      </c>
-      <c r="I8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 53</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> b- +</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> OF [/O1L[20</t>
-        </is>
-      </c>
-      <c r="B9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 59</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> AS</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> he</t>
-        </is>
-      </c>
-      <c r="F9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="G9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="H9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> LS</t>
-        </is>
-      </c>
-      <c r="I9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 64</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 54</t>
+          <t xml:space="preserve"> §). 3]</t>
         </is>
       </c>
     </row>

</xml_diff>